<commit_message>
fix warning due to update to new R version
</commit_message>
<xml_diff>
--- a/inst/extdata/james-base-settings.xlsx
+++ b/inst/extdata/james-base-settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james/ext/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8063BD6-C78C-694E-9738-5925A3BE9796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F2B0C6-7105-CF4D-9DA7-E3A11A537C3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{103B72D2-3FCD-BA4B-9A05-486FC3E56C00}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{103B72D2-3FCD-BA4B-9A05-486FC3E56C00}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="1" r:id="rId1"/>
@@ -4135,9 +4135,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AE411"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5847,7 +5847,7 @@
         <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>166</v>
+        <v>203</v>
       </c>
       <c r="C102" t="s">
         <v>9</v>
@@ -6214,7 +6214,7 @@
         <v>593</v>
       </c>
       <c r="B125" t="s">
-        <v>166</v>
+        <v>203</v>
       </c>
       <c r="C125" t="s">
         <v>9</v>
@@ -6418,7 +6418,7 @@
         <v>826</v>
       </c>
       <c r="B138" s="43" t="s">
-        <v>166</v>
+        <v>203</v>
       </c>
       <c r="C138" s="43" t="s">
         <v>9</v>
@@ -9963,8 +9963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD7057C-15EE-3240-BABA-A5F8BA4F4CF6}">
   <dimension ref="A1:AE375"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix font for saffier
</commit_message>
<xml_diff>
--- a/inst/extdata/james-base-settings.xlsx
+++ b/inst/extdata/james-base-settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james/ext/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89C054F-2060-1D40-8572-FE1BC8F49183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E8B41C-E41E-B44A-8ABB-AA2CB6FE3CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="500" windowWidth="34560" windowHeight="21100" activeTab="1" xr2:uid="{103B72D2-3FCD-BA4B-9A05-486FC3E56C00}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2326" uniqueCount="1187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="1187">
   <si>
     <t>default</t>
   </si>
@@ -3341,9 +3341,6 @@
     <t>font_path</t>
   </si>
   <si>
-    <t>fix_path_rel("fonts", path_base = "p_james")</t>
-  </si>
-  <si>
     <t>james_sh_path</t>
   </si>
   <si>
@@ -3494,9 +3491,6 @@
     <t>Your parameters are available as p\$parameter. You have acces to your data as follows. The x-values are in p\$data[, 1]. The first time series is p\$data[, 2], the second is p\$data[, 3], etc. If you generate figures from R (*i.e.* not Excel), you may define a function 'custom &lt;- function(p) { ... }' with a custom implementation instead.</t>
   </si>
   <si>
-    <t>Gives path to font, dependent on platform (*i.e.* windows, linux, osx)</t>
-  </si>
-  <si>
     <t>/Volumes/p_james/release</t>
   </si>
   <si>
@@ -3602,7 +3596,13 @@
     <t>/nas/data</t>
   </si>
   <si>
-    <t>2022-10-04</t>
+    <t>M:/p_james/fonts, /cifs/p_james/fonts, ~/Library/Fonts, fonts</t>
+  </si>
+  <si>
+    <t>Gives path to font, dependent on platform or app (*i.e.* windows, linux, osx, shiny app)</t>
+  </si>
+  <si>
+    <t>2022-11-02</t>
   </si>
 </sst>
 </file>
@@ -4217,7 +4217,7 @@
   <dimension ref="A1:AE419"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
@@ -4568,7 +4568,7 @@
         <v>951</v>
       </c>
       <c r="AB15" s="5" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="AC15" s="3" t="s">
         <v>55</v>
@@ -5135,7 +5135,7 @@
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
@@ -5146,7 +5146,7 @@
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -5191,16 +5191,19 @@
         <v>1098</v>
       </c>
       <c r="B52" t="s">
-        <v>1095</v>
+        <v>117</v>
+      </c>
+      <c r="C52" t="s">
+        <v>426</v>
       </c>
       <c r="E52" t="s">
-        <v>1099</v>
+        <v>1184</v>
       </c>
       <c r="AB52" t="s">
         <v>427</v>
       </c>
       <c r="AC52" t="s">
-        <v>1150</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.2">
@@ -6423,7 +6426,7 @@
         <v>601</v>
       </c>
       <c r="AD132" s="40" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="133" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.2">
@@ -6448,7 +6451,7 @@
         <v>336</v>
       </c>
       <c r="AC135" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="136" spans="1:30" x14ac:dyDescent="0.2">
@@ -6488,10 +6491,10 @@
         <v>72</v>
       </c>
       <c r="AC137" s="43" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="AD137" s="43" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="138" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
@@ -6505,10 +6508,10 @@
         <v>9</v>
       </c>
       <c r="AC138" s="43" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="AD138" s="44" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="139" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
@@ -6530,7 +6533,7 @@
     </row>
     <row r="140" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="42" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B140" s="43" t="s">
         <v>10</v>
@@ -6539,7 +6542,7 @@
         <v>2</v>
       </c>
       <c r="AC140" s="43" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="AD140" s="44" t="s">
         <v>830</v>
@@ -6559,7 +6562,7 @@
         <v>3</v>
       </c>
       <c r="AC141" s="43" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="142" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
@@ -6718,13 +6721,13 @@
     </row>
     <row r="152" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A152" s="8" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="AD152" s="3"/>
     </row>
     <row r="153" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="B153" t="s">
         <v>72</v>
@@ -6733,19 +6736,19 @@
         <v>15</v>
       </c>
       <c r="Z153" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="AB153" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="AC153" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="AD153" s="3"/>
     </row>
     <row r="154" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="B154" t="s">
         <v>72</v>
@@ -6757,16 +6760,16 @@
         <v>5</v>
       </c>
       <c r="AB154" t="s">
+        <v>1159</v>
+      </c>
+      <c r="AC154" t="s">
         <v>1161</v>
-      </c>
-      <c r="AC154" t="s">
-        <v>1163</v>
       </c>
       <c r="AD154" s="3"/>
     </row>
     <row r="155" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B155" t="s">
         <v>117</v>
@@ -6775,18 +6778,18 @@
         <v>72</v>
       </c>
       <c r="AB155" t="s">
+        <v>1160</v>
+      </c>
+      <c r="AC155" t="s">
         <v>1162</v>
       </c>
-      <c r="AC155" t="s">
-        <v>1164</v>
-      </c>
       <c r="AD155" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="156" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="B156" t="s">
         <v>117</v>
@@ -6798,18 +6801,18 @@
         <v>885</v>
       </c>
       <c r="AB156" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="AC156" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="AD156" s="3" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="157" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="B157" t="s">
         <v>117</v>
@@ -6818,16 +6821,16 @@
         <v>9</v>
       </c>
       <c r="AB157" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="AC157" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="AD157" s="3"/>
     </row>
     <row r="158" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="B158" t="s">
         <v>588</v>
@@ -6949,7 +6952,7 @@
         <v>210</v>
       </c>
       <c r="AC168" s="6" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="AD168" s="6"/>
     </row>
@@ -7089,7 +7092,7 @@
         <v>2</v>
       </c>
       <c r="AC180" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="AD180" t="s">
         <v>181</v>
@@ -7338,7 +7341,7 @@
         <v>10</v>
       </c>
       <c r="AC201" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="202" spans="1:31" x14ac:dyDescent="0.2">
@@ -7350,7 +7353,7 @@
       </c>
       <c r="AB202" s="5"/>
       <c r="AC202" s="3" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="AD202" s="3"/>
     </row>
@@ -7724,7 +7727,7 @@
         <v>197</v>
       </c>
       <c r="AC234" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="235" spans="1:29" x14ac:dyDescent="0.2">
@@ -7912,7 +7915,7 @@
       <c r="I245" s="5"/>
       <c r="J245" s="5"/>
       <c r="AD245" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="246" spans="1:30" x14ac:dyDescent="0.2">
@@ -7999,7 +8002,7 @@
         <v>917</v>
       </c>
       <c r="AC255" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="260" spans="1:30" x14ac:dyDescent="0.2">
@@ -8033,7 +8036,7 @@
     </row>
     <row r="262" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="B262" t="s">
         <v>10</v>
@@ -8042,10 +8045,10 @@
         <v>3</v>
       </c>
       <c r="AB262" s="5" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="AC262" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="263" spans="1:30" x14ac:dyDescent="0.2">
@@ -9715,15 +9718,15 @@
         <v>957</v>
       </c>
       <c r="AC374" s="3" t="s">
+        <v>1123</v>
+      </c>
+      <c r="AD374" t="s">
         <v>1124</v>
-      </c>
-      <c r="AD374" t="s">
-        <v>1125</v>
       </c>
     </row>
     <row r="375" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B375" t="s">
         <v>10</v>
@@ -9733,7 +9736,7 @@
       </c>
       <c r="AB375" s="5"/>
       <c r="AC375" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="AD375" s="3" t="s">
         <v>448</v>
@@ -10086,10 +10089,10 @@
     </row>
     <row r="404" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A404" s="8" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="AC404" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="405" spans="1:30" x14ac:dyDescent="0.2">
@@ -10133,7 +10136,7 @@
     </row>
     <row r="408" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A408" s="6" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B408" t="s">
         <v>10</v>
@@ -10142,12 +10145,12 @@
         <v>3</v>
       </c>
       <c r="AC408" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="409" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B409" t="s">
         <v>9</v>
@@ -10156,7 +10159,7 @@
         <v>3</v>
       </c>
       <c r="AC409" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="411" spans="1:30" x14ac:dyDescent="0.2">
@@ -10319,7 +10322,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="AC3" t="s">
         <v>1058</v>
@@ -10418,7 +10421,7 @@
         <v>426</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="F10"/>
       <c r="AA10" s="33" t="s">
@@ -10433,7 +10436,7 @@
         <v>426</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="F11"/>
       <c r="AA11" s="33" t="s">
@@ -10448,7 +10451,7 @@
         <v>426</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="F12"/>
     </row>
@@ -10485,7 +10488,7 @@
     </row>
     <row r="15" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="33" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B15" s="33" t="s">
         <v>9</v>
@@ -10493,13 +10496,13 @@
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="F15"/>
     </row>
     <row r="16" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B16" t="s">
         <v>1095</v>
@@ -10507,13 +10510,13 @@
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="F16"/>
     </row>
     <row r="17" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B17" t="s">
         <v>1095</v>
@@ -10521,13 +10524,13 @@
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="F17"/>
     </row>
     <row r="18" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -10535,13 +10538,13 @@
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="F18"/>
     </row>
     <row r="19" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B19" t="s">
         <v>1095</v>
@@ -10549,7 +10552,7 @@
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="F19"/>
     </row>
@@ -10564,7 +10567,7 @@
         <v>426</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="F20"/>
       <c r="AA20" s="33" t="s">
@@ -10670,7 +10673,7 @@
         <v>426</v>
       </c>
       <c r="E26" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
@@ -10692,62 +10695,62 @@
         <v>426</v>
       </c>
       <c r="E28" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B30" t="s">
         <v>1095</v>
       </c>
       <c r="E30" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B31" t="s">
         <v>1095</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="B32" t="s">
         <v>1095</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="B34" t="s">
         <v>1095</v>
       </c>
       <c r="E34" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="57" spans="6:6" x14ac:dyDescent="0.2">
@@ -10956,7 +10959,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="AC3" t="s">
         <v>91</v>
@@ -12107,7 +12110,7 @@
   <dimension ref="A1:AE31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13576,7 +13579,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="AA22" t="s">
         <v>3</v>
@@ -13590,7 +13593,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="AA23" t="s">
         <v>3</v>
@@ -13598,7 +13601,7 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B24" t="s">
         <v>117</v>
@@ -13607,7 +13610,7 @@
         <v>426</v>
       </c>
       <c r="E24" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="AA24" t="s">
         <v>3</v>
@@ -13615,24 +13618,24 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
         <v>1182</v>
-      </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" t="s">
-        <v>1184</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>